<commit_message>
checked if user left password empty
</commit_message>
<xml_diff>
--- a/accounts.xlsx
+++ b/accounts.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="4">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="9">
   <si>
     <t>password</t>
   </si>
@@ -22,10 +22,25 @@
     <t>balance</t>
   </si>
   <si>
+    <t>username</t>
+  </si>
+  <si>
     <t>sumona</t>
   </si>
   <si>
-    <t>12345</t>
+    <t>sarmin</t>
+  </si>
+  <si>
+    <t>ria</t>
+  </si>
+  <si>
+    <t>123</t>
+  </si>
+  <si>
+    <t>nan</t>
+  </si>
+  <si>
+    <t>89</t>
   </si>
 </sst>
 </file>
@@ -383,13 +398,16 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:C2"/>
+  <dimension ref="A1:C4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
     <row r="1" spans="1:3">
+      <c r="A1" s="1" t="s">
+        <v>2</v>
+      </c>
       <c r="B1" s="1" t="s">
         <v>0</v>
       </c>
@@ -399,12 +417,34 @@
     </row>
     <row r="2" spans="1:3">
       <c r="A2" s="1" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="B2" t="s">
-        <v>3</v>
+        <v>6</v>
       </c>
       <c r="C2">
+        <v>988</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3">
+      <c r="A3" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="B3" t="s">
+        <v>7</v>
+      </c>
+      <c r="C3">
+        <v>1012</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3">
+      <c r="A4" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="B4" t="s">
+        <v>8</v>
+      </c>
+      <c r="C4">
         <v>1000</v>
       </c>
     </row>

</xml_diff>

<commit_message>
withdraw and deposit added
</commit_message>
<xml_diff>
--- a/accounts.xlsx
+++ b/accounts.xlsx
@@ -34,7 +34,7 @@
     <t>ria</t>
   </si>
   <si>
-    <t>123</t>
+    <t>1234</t>
   </si>
   <si>
     <t>nan</t>
@@ -423,7 +423,7 @@
         <v>6</v>
       </c>
       <c r="C2">
-        <v>988</v>
+        <v>1070</v>
       </c>
     </row>
     <row r="3" spans="1:3">

</xml_diff>